<commit_message>
add exceed button and changed data storage type
</commit_message>
<xml_diff>
--- a/TrafficToolCounting/results/Q2_TLC00024_c.xlsx
+++ b/TrafficToolCounting/results/Q2_TLC00024_c.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>L1</t>
   </si>
@@ -209,6 +209,21 @@
   </si>
   <si>
     <t>2023-04-04 15:29:31</t>
+  </si>
+  <si>
+    <t>6+</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0+</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>17+</t>
   </si>
 </sst>
 </file>
@@ -590,8 +605,8 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>65</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -604,11 +619,11 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -618,11 +633,11 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -632,14 +647,14 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>